<commit_message>
ccbottlersus, fix 3 issues
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/KPITemplateV4.1.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/KPITemplateV4.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="a" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="b" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
@@ -45,6 +46,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="a" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="b" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
@@ -57,6 +59,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SOS!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="a" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="b" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
@@ -69,6 +72,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -80,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="281">
   <si>
     <t>Region</t>
   </si>
@@ -1326,20 +1330,20 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+      <selection pane="bottomRight" activeCell="G69" activeCellId="0" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="11" min="7" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="15" min="13" style="1" width="8.67611336032389"/>
@@ -3899,6 +3903,9 @@
       <c r="F68" s="6" t="s">
         <v>172</v>
       </c>
+      <c r="G68" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H68" s="6" t="s">
         <v>170</v>
       </c>
@@ -3929,6 +3936,9 @@
       <c r="F69" s="6" t="s">
         <v>174</v>
       </c>
+      <c r="G69" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="H69" s="6" t="s">
         <v>173</v>
       </c>
@@ -3958,6 +3968,9 @@
       </c>
       <c r="F70" s="6" t="s">
         <v>176</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>175</v>
@@ -4002,7 +4015,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="13" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="1017" min="4" style="13" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.67611336032389"/>
   </cols>
@@ -21457,10 +21470,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3157894736842"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.67611336032389"/>
@@ -22056,7 +22069,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
@@ -22068,8 +22081,8 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.67611336032389"/>

</xml_diff>